<commit_message>
nächste Woche und Assignment 3
</commit_message>
<xml_diff>
--- a/Assignments/Assignment 1/Results Assignment 1 - with names.xlsx
+++ b/Assignments/Assignment 1/Results Assignment 1 - with names.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\Studium\Tutorials\Tutorat ISM\Survey_Tutorial_24_25\Assignments\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bache\Documents\Studium&amp;Beruf\Uni\Master\1.Semester\Survey Tut\Survey_Tutorial_24_25\Assignments\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7070A78-EFAC-4EBF-8842-8985A0C1D505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEB2157-66AE-4A1C-935E-B45E24BD9123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -291,9 +291,6 @@
     <t xml:space="preserve">Finn Krüger </t>
   </si>
   <si>
-    <t>01/1380046</t>
-  </si>
-  <si>
     <t>Maximilian Lapsin</t>
   </si>
   <si>
@@ -394,6 +391,9 @@
   </si>
   <si>
     <t>Jana Behrens</t>
+  </si>
+  <si>
+    <t>01/1380446</t>
   </si>
 </sst>
 </file>
@@ -445,8 +445,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -726,28 +726,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C61" activeCellId="1" sqref="A61 C61"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="34.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -758,7 +758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -769,7 +769,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -780,7 +780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -791,7 +791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -802,7 +802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -813,7 +813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -824,7 +824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -835,7 +835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -846,29 +846,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" t="s">
         <v>96</v>
       </c>
-      <c r="B11" t="s">
-        <v>97</v>
-      </c>
       <c r="C11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
         <v>94</v>
-      </c>
-      <c r="B12" t="s">
-        <v>95</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -879,7 +879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -890,7 +890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -901,18 +901,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="s">
         <v>114</v>
       </c>
-      <c r="B16" t="s">
-        <v>115</v>
-      </c>
       <c r="C16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -923,7 +923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -934,7 +934,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -945,7 +945,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -956,18 +956,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
         <v>90</v>
       </c>
-      <c r="B21" t="s">
-        <v>91</v>
-      </c>
       <c r="C21">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -978,7 +978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -989,7 +989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1055,9 +1055,9 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
         <v>21</v>
@@ -1066,7 +1066,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -1088,18 +1088,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
         <v>98</v>
       </c>
-      <c r="B33" t="s">
-        <v>99</v>
-      </c>
       <c r="C33">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -1110,18 +1110,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" t="s">
         <v>108</v>
       </c>
-      <c r="B35" t="s">
-        <v>109</v>
-      </c>
       <c r="C35">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -1143,29 +1143,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
         <v>92</v>
       </c>
-      <c r="B38" t="s">
-        <v>93</v>
-      </c>
       <c r="C38">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" t="s">
         <v>88</v>
-      </c>
-      <c r="B39" t="s">
-        <v>89</v>
       </c>
       <c r="C39">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -1187,18 +1187,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" t="s">
         <v>116</v>
-      </c>
-      <c r="B42" t="s">
-        <v>117</v>
       </c>
       <c r="C42">
         <v>6.5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -1220,51 +1220,51 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" t="s">
         <v>104</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>105</v>
       </c>
-      <c r="C45">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" t="s">
-        <v>101</v>
-      </c>
-      <c r="C46">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>102</v>
-      </c>
-      <c r="B47" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>106</v>
       </c>
-      <c r="B48" t="s">
-        <v>107</v>
-      </c>
       <c r="C48">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -1275,18 +1275,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" t="s">
         <v>110</v>
       </c>
-      <c r="B50" t="s">
-        <v>111</v>
-      </c>
       <c r="C50">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>40</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>30</v>
       </c>
@@ -1319,18 +1319,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" t="s">
         <v>112</v>
       </c>
-      <c r="B54" t="s">
-        <v>113</v>
-      </c>
       <c r="C54">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>80</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -1396,12 +1396,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
         <v>121</v>
-      </c>
-      <c r="B61" t="s">
-        <v>122</v>
       </c>
       <c r="C61" s="1">
         <v>7</v>

</xml_diff>